<commit_message>
Fitness still high for some reason
</commit_message>
<xml_diff>
--- a/src/gatourism/data_P.xlsx
+++ b/src/gatourism/data_P.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="195">
   <si>
     <t>title</t>
   </si>
@@ -596,13 +596,16 @@
   </si>
   <si>
     <t>Nét Huế Restaurant</t>
+  </si>
+  <si>
+    <t>Starting point</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -612,6 +615,11 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -663,7 +671,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -687,6 +695,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -990,10 +1007,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F190"/>
+  <dimension ref="A1:F191"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A161" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A190"/>
+    <sheetView tabSelected="1" topLeftCell="A166" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A191"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1023,20 +1040,20 @@
       <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="6">
-        <v>28800</v>
-      </c>
-      <c r="D2">
-        <v>81000</v>
-      </c>
-      <c r="E2" s="6">
-        <v>273188</v>
-      </c>
-      <c r="F2">
-        <v>7200</v>
+      <c r="B2" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="C2" s="11">
+        <v>0</v>
+      </c>
+      <c r="D2" s="10">
+        <v>0</v>
+      </c>
+      <c r="E2" s="10">
+        <v>0</v>
+      </c>
+      <c r="F2" s="12">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -1044,16 +1061,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" s="6">
-        <v>25200</v>
+        <v>28800</v>
       </c>
       <c r="D3">
-        <v>77400</v>
+        <v>81000</v>
       </c>
       <c r="E3" s="6">
-        <v>285057</v>
+        <v>273188</v>
       </c>
       <c r="F3">
         <v>7200</v>
@@ -1064,16 +1081,16 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" s="6">
-        <v>32400</v>
+        <v>25200</v>
       </c>
       <c r="D4">
         <v>77400</v>
       </c>
       <c r="E4" s="6">
-        <v>122690</v>
+        <v>285057</v>
       </c>
       <c r="F4">
         <v>7200</v>
@@ -1084,16 +1101,16 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5" s="6">
-        <v>30600</v>
+        <v>32400</v>
       </c>
       <c r="D5">
-        <v>63000</v>
+        <v>77400</v>
       </c>
       <c r="E5" s="6">
-        <v>267071</v>
+        <v>122690</v>
       </c>
       <c r="F5">
         <v>7200</v>
@@ -1104,16 +1121,16 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C6" s="6">
-        <v>28800</v>
+        <v>30600</v>
       </c>
       <c r="D6">
-        <v>77400</v>
+        <v>63000</v>
       </c>
       <c r="E6" s="6">
-        <v>144241</v>
+        <v>267071</v>
       </c>
       <c r="F6">
         <v>7200</v>
@@ -1124,16 +1141,16 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C7" s="6">
-        <v>34200</v>
+        <v>28800</v>
       </c>
       <c r="D7">
-        <v>63000</v>
+        <v>77400</v>
       </c>
       <c r="E7" s="6">
-        <v>206336</v>
+        <v>144241</v>
       </c>
       <c r="F7">
         <v>7200</v>
@@ -1144,16 +1161,16 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C8" s="6">
-        <v>30600</v>
+        <v>34200</v>
       </c>
       <c r="D8">
         <v>63000</v>
       </c>
       <c r="E8" s="6">
-        <v>207468</v>
+        <v>206336</v>
       </c>
       <c r="F8">
         <v>7200</v>
@@ -1164,16 +1181,16 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="7">
-        <v>28800</v>
-      </c>
-      <c r="D9" s="3">
-        <v>41400</v>
+        <v>11</v>
+      </c>
+      <c r="C9" s="6">
+        <v>30600</v>
+      </c>
+      <c r="D9">
+        <v>63000</v>
       </c>
       <c r="E9" s="6">
-        <v>146196</v>
+        <v>207468</v>
       </c>
       <c r="F9">
         <v>7200</v>
@@ -1184,16 +1201,16 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="6">
-        <v>30600</v>
-      </c>
-      <c r="D10">
-        <v>61200</v>
+        <v>12</v>
+      </c>
+      <c r="C10" s="7">
+        <v>28800</v>
+      </c>
+      <c r="D10" s="3">
+        <v>41400</v>
       </c>
       <c r="E10" s="6">
-        <v>129415</v>
+        <v>146196</v>
       </c>
       <c r="F10">
         <v>7200</v>
@@ -1204,16 +1221,16 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C11" s="6">
-        <v>25200</v>
+        <v>30600</v>
       </c>
       <c r="D11">
-        <v>77400</v>
+        <v>61200</v>
       </c>
       <c r="E11" s="6">
-        <v>178695</v>
+        <v>129415</v>
       </c>
       <c r="F11">
         <v>7200</v>
@@ -1224,16 +1241,16 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C12" s="6">
         <v>25200</v>
       </c>
       <c r="D12">
-        <v>75600</v>
+        <v>77400</v>
       </c>
       <c r="E12" s="6">
-        <v>221641</v>
+        <v>178695</v>
       </c>
       <c r="F12">
         <v>7200</v>
@@ -1244,16 +1261,16 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C13" s="6">
         <v>25200</v>
       </c>
       <c r="D13">
-        <v>43200</v>
+        <v>75600</v>
       </c>
       <c r="E13" s="6">
-        <v>225617</v>
+        <v>221641</v>
       </c>
       <c r="F13">
         <v>7200</v>
@@ -1264,16 +1281,16 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C14" s="6">
         <v>25200</v>
       </c>
       <c r="D14">
-        <v>77400</v>
+        <v>43200</v>
       </c>
       <c r="E14" s="6">
-        <v>222973</v>
+        <v>225617</v>
       </c>
       <c r="F14">
         <v>7200</v>
@@ -1284,16 +1301,16 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C15" s="6">
-        <v>28800</v>
+        <v>25200</v>
       </c>
       <c r="D15">
-        <v>79200</v>
+        <v>77400</v>
       </c>
       <c r="E15" s="6">
-        <v>209177</v>
+        <v>222973</v>
       </c>
       <c r="F15">
         <v>7200</v>
@@ -1304,16 +1321,16 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C16" s="6">
-        <v>46800</v>
+        <v>28800</v>
       </c>
       <c r="D16">
         <v>79200</v>
       </c>
       <c r="E16" s="6">
-        <v>178743</v>
+        <v>209177</v>
       </c>
       <c r="F16">
         <v>7200</v>
@@ -1324,16 +1341,16 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C17" s="6">
-        <v>30600</v>
+        <v>46800</v>
       </c>
       <c r="D17">
         <v>79200</v>
       </c>
       <c r="E17" s="6">
-        <v>169066</v>
+        <v>178743</v>
       </c>
       <c r="F17">
         <v>7200</v>
@@ -1344,16 +1361,16 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C18" s="6">
-        <v>28800</v>
+        <v>30600</v>
       </c>
       <c r="D18">
-        <v>75600</v>
+        <v>79200</v>
       </c>
       <c r="E18" s="6">
-        <v>179159</v>
+        <v>169066</v>
       </c>
       <c r="F18">
         <v>7200</v>
@@ -1364,16 +1381,16 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C19" s="6">
-        <v>30600</v>
+        <v>28800</v>
       </c>
       <c r="D19">
-        <v>72000</v>
+        <v>75600</v>
       </c>
       <c r="E19" s="6">
-        <v>196029</v>
+        <v>179159</v>
       </c>
       <c r="F19">
         <v>7200</v>
@@ -1384,16 +1401,16 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C20" s="6">
-        <v>28800</v>
+        <v>30600</v>
       </c>
       <c r="D20">
-        <v>64800</v>
+        <v>72000</v>
       </c>
       <c r="E20" s="6">
-        <v>234540</v>
+        <v>196029</v>
       </c>
       <c r="F20">
         <v>7200</v>
@@ -1404,16 +1421,16 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C21" s="6">
-        <v>25200</v>
+        <v>28800</v>
       </c>
       <c r="D21">
-        <v>61200</v>
+        <v>64800</v>
       </c>
       <c r="E21" s="6">
-        <v>245751</v>
+        <v>234540</v>
       </c>
       <c r="F21">
         <v>7200</v>
@@ -1424,16 +1441,16 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C22" s="6">
-        <v>30600</v>
+        <v>25200</v>
       </c>
       <c r="D22">
-        <v>72000</v>
+        <v>61200</v>
       </c>
       <c r="E22" s="6">
-        <v>113699</v>
+        <v>245751</v>
       </c>
       <c r="F22">
         <v>7200</v>
@@ -1444,16 +1461,16 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C23" s="6">
-        <v>28800</v>
+        <v>30600</v>
       </c>
       <c r="D23">
-        <v>75600</v>
+        <v>72000</v>
       </c>
       <c r="E23" s="6">
-        <v>216224</v>
+        <v>113699</v>
       </c>
       <c r="F23">
         <v>7200</v>
@@ -1464,16 +1481,16 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C24" s="6">
-        <v>25200</v>
+        <v>28800</v>
       </c>
       <c r="D24">
-        <v>64800</v>
+        <v>75600</v>
       </c>
       <c r="E24" s="6">
-        <v>115547</v>
+        <v>216224</v>
       </c>
       <c r="F24">
         <v>7200</v>
@@ -1484,16 +1501,16 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C25" s="6">
-        <v>28800</v>
+        <v>25200</v>
       </c>
       <c r="D25">
-        <v>75600</v>
+        <v>64800</v>
       </c>
       <c r="E25" s="6">
-        <v>180930</v>
+        <v>115547</v>
       </c>
       <c r="F25">
         <v>7200</v>
@@ -1504,16 +1521,16 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C26" s="6">
-        <v>30600</v>
+        <v>28800</v>
       </c>
       <c r="D26">
-        <v>72000</v>
+        <v>75600</v>
       </c>
       <c r="E26" s="6">
-        <v>248581</v>
+        <v>180930</v>
       </c>
       <c r="F26">
         <v>7200</v>
@@ -1524,16 +1541,16 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>30</v>
-      </c>
-      <c r="C27" s="8">
-        <v>0</v>
-      </c>
-      <c r="D27" s="8">
-        <v>86400</v>
+        <v>29</v>
+      </c>
+      <c r="C27" s="6">
+        <v>30600</v>
+      </c>
+      <c r="D27">
+        <v>72000</v>
       </c>
       <c r="E27" s="6">
-        <v>233807</v>
+        <v>248581</v>
       </c>
       <c r="F27">
         <v>7200</v>
@@ -1544,16 +1561,16 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>31</v>
-      </c>
-      <c r="C28" s="6">
-        <v>28800</v>
-      </c>
-      <c r="D28">
-        <v>75600</v>
+        <v>30</v>
+      </c>
+      <c r="C28" s="8">
+        <v>0</v>
+      </c>
+      <c r="D28" s="8">
+        <v>86400</v>
       </c>
       <c r="E28" s="6">
-        <v>211010</v>
+        <v>233807</v>
       </c>
       <c r="F28">
         <v>7200</v>
@@ -1564,16 +1581,16 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C29" s="6">
         <v>28800</v>
       </c>
       <c r="D29">
-        <v>57600</v>
+        <v>75600</v>
       </c>
       <c r="E29" s="6">
-        <v>217316</v>
+        <v>211010</v>
       </c>
       <c r="F29">
         <v>7200</v>
@@ -1584,16 +1601,16 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C30" s="6">
         <v>28800</v>
       </c>
       <c r="D30">
-        <v>75600</v>
+        <v>57600</v>
       </c>
       <c r="E30" s="6">
-        <v>124842</v>
+        <v>217316</v>
       </c>
       <c r="F30">
         <v>7200</v>
@@ -1604,16 +1621,16 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C31" s="6">
         <v>28800</v>
       </c>
       <c r="D31">
-        <v>81000</v>
+        <v>75600</v>
       </c>
       <c r="E31" s="6">
-        <v>298020</v>
+        <v>124842</v>
       </c>
       <c r="F31">
         <v>7200</v>
@@ -1624,16 +1641,16 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C32" s="6">
         <v>28800</v>
       </c>
       <c r="D32">
-        <v>77400</v>
+        <v>81000</v>
       </c>
       <c r="E32" s="6">
-        <v>121574</v>
+        <v>298020</v>
       </c>
       <c r="F32">
         <v>7200</v>
@@ -1644,7 +1661,7 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C33" s="6">
         <v>28800</v>
@@ -1653,7 +1670,7 @@
         <v>77400</v>
       </c>
       <c r="E33" s="6">
-        <v>298040</v>
+        <v>121574</v>
       </c>
       <c r="F33">
         <v>7200</v>
@@ -1664,16 +1681,16 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C34" s="6">
-        <v>32400</v>
+        <v>28800</v>
       </c>
       <c r="D34">
         <v>77400</v>
       </c>
       <c r="E34" s="6">
-        <v>230123</v>
+        <v>298040</v>
       </c>
       <c r="F34">
         <v>7200</v>
@@ -1684,16 +1701,16 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C35" s="6">
-        <v>28800</v>
+        <v>32400</v>
       </c>
       <c r="D35">
-        <v>79200</v>
+        <v>77400</v>
       </c>
       <c r="E35" s="6">
-        <v>172690</v>
+        <v>230123</v>
       </c>
       <c r="F35">
         <v>7200</v>
@@ -1704,16 +1721,16 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C36" s="6">
-        <v>25200</v>
+        <v>28800</v>
       </c>
       <c r="D36">
-        <v>43200</v>
+        <v>79200</v>
       </c>
       <c r="E36" s="6">
-        <v>183633</v>
+        <v>172690</v>
       </c>
       <c r="F36">
         <v>7200</v>
@@ -1724,16 +1741,16 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C37" s="6">
-        <v>28800</v>
+        <v>25200</v>
       </c>
       <c r="D37">
-        <v>75600</v>
+        <v>43200</v>
       </c>
       <c r="E37" s="6">
-        <v>224211</v>
+        <v>183633</v>
       </c>
       <c r="F37">
         <v>7200</v>
@@ -1744,16 +1761,16 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C38" s="6">
-        <v>32400</v>
+        <v>28800</v>
       </c>
       <c r="D38">
-        <v>63000</v>
+        <v>75600</v>
       </c>
       <c r="E38" s="6">
-        <v>132034</v>
+        <v>224211</v>
       </c>
       <c r="F38">
         <v>7200</v>
@@ -1764,16 +1781,16 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C39" s="6">
-        <v>28800</v>
+        <v>32400</v>
       </c>
       <c r="D39">
-        <v>64800</v>
+        <v>63000</v>
       </c>
       <c r="E39" s="6">
-        <v>290535</v>
+        <v>132034</v>
       </c>
       <c r="F39">
         <v>7200</v>
@@ -1784,16 +1801,16 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C40" s="6">
         <v>28800</v>
       </c>
       <c r="D40">
-        <v>61200</v>
+        <v>64800</v>
       </c>
       <c r="E40" s="6">
-        <v>128671</v>
+        <v>290535</v>
       </c>
       <c r="F40">
         <v>7200</v>
@@ -1804,16 +1821,16 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C41" s="6">
-        <v>30600</v>
+        <v>28800</v>
       </c>
       <c r="D41">
-        <v>63000</v>
+        <v>61200</v>
       </c>
       <c r="E41" s="6">
-        <v>242301</v>
+        <v>128671</v>
       </c>
       <c r="F41">
         <v>7200</v>
@@ -1824,16 +1841,16 @@
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>45</v>
-      </c>
-      <c r="C42" s="8">
-        <v>0</v>
-      </c>
-      <c r="D42" s="8">
-        <v>86400</v>
+        <v>44</v>
+      </c>
+      <c r="C42" s="6">
+        <v>30600</v>
+      </c>
+      <c r="D42">
+        <v>63000</v>
       </c>
       <c r="E42" s="6">
-        <v>173391</v>
+        <v>242301</v>
       </c>
       <c r="F42">
         <v>7200</v>
@@ -1844,16 +1861,16 @@
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>46</v>
-      </c>
-      <c r="C43" s="6">
-        <v>25200</v>
-      </c>
-      <c r="D43">
-        <v>61200</v>
+        <v>45</v>
+      </c>
+      <c r="C43" s="8">
+        <v>0</v>
+      </c>
+      <c r="D43" s="8">
+        <v>86400</v>
       </c>
       <c r="E43" s="6">
-        <v>222515</v>
+        <v>173391</v>
       </c>
       <c r="F43">
         <v>7200</v>
@@ -1864,16 +1881,16 @@
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C44" s="6">
-        <v>32400</v>
+        <v>25200</v>
       </c>
       <c r="D44">
-        <v>75600</v>
+        <v>61200</v>
       </c>
       <c r="E44" s="6">
-        <v>137717</v>
+        <v>222515</v>
       </c>
       <c r="F44">
         <v>7200</v>
@@ -1884,16 +1901,16 @@
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C45" s="6">
-        <v>28800</v>
+        <v>32400</v>
       </c>
       <c r="D45">
-        <v>79200</v>
+        <v>75600</v>
       </c>
       <c r="E45" s="6">
-        <v>212968</v>
+        <v>137717</v>
       </c>
       <c r="F45">
         <v>7200</v>
@@ -1904,7 +1921,7 @@
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C46" s="6">
         <v>28800</v>
@@ -1913,7 +1930,7 @@
         <v>79200</v>
       </c>
       <c r="E46" s="6">
-        <v>120022</v>
+        <v>212968</v>
       </c>
       <c r="F46">
         <v>7200</v>
@@ -1924,16 +1941,16 @@
         <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C47" s="6">
-        <v>25200</v>
+        <v>28800</v>
       </c>
       <c r="D47">
         <v>79200</v>
       </c>
       <c r="E47" s="6">
-        <v>130734</v>
+        <v>120022</v>
       </c>
       <c r="F47">
         <v>7200</v>
@@ -1944,16 +1961,16 @@
         <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C48" s="6">
-        <v>23400</v>
+        <v>25200</v>
       </c>
       <c r="D48">
-        <v>77400</v>
+        <v>79200</v>
       </c>
       <c r="E48" s="6">
-        <v>143186</v>
+        <v>130734</v>
       </c>
       <c r="F48">
         <v>7200</v>
@@ -1964,16 +1981,16 @@
         <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C49" s="6">
-        <v>25200</v>
+        <v>23400</v>
       </c>
       <c r="D49">
         <v>77400</v>
       </c>
       <c r="E49" s="6">
-        <v>227969</v>
+        <v>143186</v>
       </c>
       <c r="F49">
         <v>7200</v>
@@ -1984,16 +2001,16 @@
         <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C50" s="6">
-        <v>34200</v>
+        <v>25200</v>
       </c>
       <c r="D50">
-        <v>79200</v>
+        <v>77400</v>
       </c>
       <c r="E50" s="6">
-        <v>202637</v>
+        <v>227969</v>
       </c>
       <c r="F50">
         <v>7200</v>
@@ -2004,16 +2021,16 @@
         <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C51" s="6">
-        <v>28800</v>
+        <v>34200</v>
       </c>
       <c r="D51">
-        <v>77400</v>
+        <v>79200</v>
       </c>
       <c r="E51" s="6">
-        <v>159022</v>
+        <v>202637</v>
       </c>
       <c r="F51">
         <v>7200</v>
@@ -2024,16 +2041,16 @@
         <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C52" s="6">
         <v>28800</v>
       </c>
       <c r="D52">
-        <v>63000</v>
+        <v>77400</v>
       </c>
       <c r="E52" s="6">
-        <v>122798</v>
+        <v>159022</v>
       </c>
       <c r="F52">
         <v>7200</v>
@@ -2044,16 +2061,16 @@
         <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C53" s="6">
-        <v>25200</v>
+        <v>28800</v>
       </c>
       <c r="D53">
-        <v>64800</v>
+        <v>63000</v>
       </c>
       <c r="E53" s="6">
-        <v>147087</v>
+        <v>122798</v>
       </c>
       <c r="F53">
         <v>7200</v>
@@ -2064,16 +2081,16 @@
         <v>52</v>
       </c>
       <c r="B54" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C54" s="6">
-        <v>30600</v>
+        <v>25200</v>
       </c>
       <c r="D54">
-        <v>59400</v>
+        <v>64800</v>
       </c>
       <c r="E54" s="6">
-        <v>187907</v>
+        <v>147087</v>
       </c>
       <c r="F54">
         <v>7200</v>
@@ -2084,16 +2101,16 @@
         <v>53</v>
       </c>
       <c r="B55" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C55" s="6">
-        <v>28800</v>
+        <v>30600</v>
       </c>
       <c r="D55">
-        <v>79200</v>
+        <v>59400</v>
       </c>
       <c r="E55" s="6">
-        <v>123991</v>
+        <v>187907</v>
       </c>
       <c r="F55">
         <v>7200</v>
@@ -2104,16 +2121,16 @@
         <v>54</v>
       </c>
       <c r="B56" t="s">
-        <v>59</v>
-      </c>
-      <c r="C56" s="8">
-        <v>0</v>
-      </c>
-      <c r="D56" s="8">
-        <v>86400</v>
+        <v>58</v>
+      </c>
+      <c r="C56" s="6">
+        <v>28800</v>
+      </c>
+      <c r="D56">
+        <v>79200</v>
       </c>
       <c r="E56" s="6">
-        <v>128167</v>
+        <v>123991</v>
       </c>
       <c r="F56">
         <v>7200</v>
@@ -2124,16 +2141,16 @@
         <v>55</v>
       </c>
       <c r="B57" t="s">
-        <v>60</v>
-      </c>
-      <c r="C57" s="6">
-        <v>25200</v>
-      </c>
-      <c r="D57">
-        <v>64800</v>
+        <v>59</v>
+      </c>
+      <c r="C57" s="8">
+        <v>0</v>
+      </c>
+      <c r="D57" s="8">
+        <v>86400</v>
       </c>
       <c r="E57" s="6">
-        <v>285138</v>
+        <v>128167</v>
       </c>
       <c r="F57">
         <v>7200</v>
@@ -2144,16 +2161,16 @@
         <v>56</v>
       </c>
       <c r="B58" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C58" s="6">
-        <v>28800</v>
+        <v>25200</v>
       </c>
       <c r="D58">
-        <v>61200</v>
+        <v>64800</v>
       </c>
       <c r="E58" s="6">
-        <v>173867</v>
+        <v>285138</v>
       </c>
       <c r="F58">
         <v>7200</v>
@@ -2164,16 +2181,16 @@
         <v>57</v>
       </c>
       <c r="B59" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C59" s="6">
-        <v>32400</v>
+        <v>28800</v>
       </c>
       <c r="D59">
-        <v>79200</v>
+        <v>61200</v>
       </c>
       <c r="E59" s="6">
-        <v>109660</v>
+        <v>173867</v>
       </c>
       <c r="F59">
         <v>7200</v>
@@ -2184,16 +2201,16 @@
         <v>58</v>
       </c>
       <c r="B60" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C60" s="6">
         <v>32400</v>
       </c>
       <c r="D60">
-        <v>77400</v>
+        <v>79200</v>
       </c>
       <c r="E60" s="6">
-        <v>255730</v>
+        <v>109660</v>
       </c>
       <c r="F60">
         <v>7200</v>
@@ -2204,16 +2221,16 @@
         <v>59</v>
       </c>
       <c r="B61" t="s">
-        <v>64</v>
-      </c>
-      <c r="C61" s="8">
-        <v>0</v>
-      </c>
-      <c r="D61" s="8">
-        <v>86400</v>
+        <v>63</v>
+      </c>
+      <c r="C61" s="6">
+        <v>32400</v>
+      </c>
+      <c r="D61">
+        <v>77400</v>
       </c>
       <c r="E61" s="6">
-        <v>133033</v>
+        <v>255730</v>
       </c>
       <c r="F61">
         <v>7200</v>
@@ -2224,16 +2241,16 @@
         <v>60</v>
       </c>
       <c r="B62" t="s">
-        <v>65</v>
-      </c>
-      <c r="C62" s="6">
-        <v>28800</v>
-      </c>
-      <c r="D62">
-        <v>79200</v>
+        <v>64</v>
+      </c>
+      <c r="C62" s="8">
+        <v>0</v>
+      </c>
+      <c r="D62" s="8">
+        <v>86400</v>
       </c>
       <c r="E62" s="6">
-        <v>287742</v>
+        <v>133033</v>
       </c>
       <c r="F62">
         <v>7200</v>
@@ -2244,16 +2261,16 @@
         <v>61</v>
       </c>
       <c r="B63" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C63" s="6">
-        <v>32400</v>
+        <v>28800</v>
       </c>
       <c r="D63">
-        <v>77400</v>
+        <v>79200</v>
       </c>
       <c r="E63" s="6">
-        <v>222491</v>
+        <v>287742</v>
       </c>
       <c r="F63">
         <v>7200</v>
@@ -2264,16 +2281,16 @@
         <v>62</v>
       </c>
       <c r="B64" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C64" s="6">
         <v>32400</v>
       </c>
       <c r="D64">
-        <v>84600</v>
+        <v>77400</v>
       </c>
       <c r="E64" s="6">
-        <v>229775</v>
+        <v>222491</v>
       </c>
       <c r="F64">
         <v>7200</v>
@@ -2284,16 +2301,16 @@
         <v>63</v>
       </c>
       <c r="B65" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C65" s="6">
-        <v>28800</v>
+        <v>32400</v>
       </c>
       <c r="D65">
-        <v>63000</v>
+        <v>84600</v>
       </c>
       <c r="E65" s="6">
-        <v>191148</v>
+        <v>229775</v>
       </c>
       <c r="F65">
         <v>7200</v>
@@ -2304,16 +2321,16 @@
         <v>64</v>
       </c>
       <c r="B66" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C66" s="6">
-        <v>25200</v>
+        <v>28800</v>
       </c>
       <c r="D66">
-        <v>61200</v>
+        <v>63000</v>
       </c>
       <c r="E66" s="6">
-        <v>196655</v>
+        <v>191148</v>
       </c>
       <c r="F66">
         <v>7200</v>
@@ -2324,16 +2341,16 @@
         <v>65</v>
       </c>
       <c r="B67" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C67" s="6">
-        <v>18000</v>
+        <v>25200</v>
       </c>
       <c r="D67">
-        <v>79200</v>
+        <v>61200</v>
       </c>
       <c r="E67" s="6">
-        <v>205599</v>
+        <v>196655</v>
       </c>
       <c r="F67">
         <v>7200</v>
@@ -2344,16 +2361,16 @@
         <v>66</v>
       </c>
       <c r="B68" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C68" s="6">
-        <v>25200</v>
+        <v>18000</v>
       </c>
       <c r="D68">
-        <v>64800</v>
+        <v>79200</v>
       </c>
       <c r="E68" s="6">
-        <v>123976</v>
+        <v>205599</v>
       </c>
       <c r="F68">
         <v>7200</v>
@@ -2364,16 +2381,16 @@
         <v>67</v>
       </c>
       <c r="B69" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C69" s="6">
-        <v>0</v>
+        <v>25200</v>
       </c>
       <c r="D69">
-        <v>86400</v>
+        <v>64800</v>
       </c>
       <c r="E69" s="6">
-        <v>262620</v>
+        <v>123976</v>
       </c>
       <c r="F69">
         <v>7200</v>
@@ -2384,16 +2401,16 @@
         <v>68</v>
       </c>
       <c r="B70" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C70" s="6">
-        <v>27000</v>
+        <v>0</v>
       </c>
       <c r="D70">
-        <v>79200</v>
+        <v>86400</v>
       </c>
       <c r="E70" s="6">
-        <v>273732</v>
+        <v>262620</v>
       </c>
       <c r="F70">
         <v>7200</v>
@@ -2404,16 +2421,16 @@
         <v>69</v>
       </c>
       <c r="B71" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C71" s="6">
-        <v>28800</v>
+        <v>27000</v>
       </c>
       <c r="D71">
-        <v>61200</v>
+        <v>79200</v>
       </c>
       <c r="E71" s="6">
-        <v>140022</v>
+        <v>273732</v>
       </c>
       <c r="F71">
         <v>7200</v>
@@ -2424,16 +2441,16 @@
         <v>70</v>
       </c>
       <c r="B72" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C72" s="6">
-        <v>21600</v>
+        <v>28800</v>
       </c>
       <c r="D72">
-        <v>81000</v>
+        <v>61200</v>
       </c>
       <c r="E72" s="6">
-        <v>130457</v>
+        <v>140022</v>
       </c>
       <c r="F72">
         <v>7200</v>
@@ -2444,16 +2461,16 @@
         <v>71</v>
       </c>
       <c r="B73" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C73" s="6">
-        <v>27000</v>
+        <v>21600</v>
       </c>
       <c r="D73">
-        <v>77400</v>
+        <v>81000</v>
       </c>
       <c r="E73" s="6">
-        <v>176534</v>
+        <v>130457</v>
       </c>
       <c r="F73">
         <v>7200</v>
@@ -2464,16 +2481,16 @@
         <v>72</v>
       </c>
       <c r="B74" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C74" s="6">
-        <v>28800</v>
+        <v>27000</v>
       </c>
       <c r="D74">
-        <v>79200</v>
+        <v>77400</v>
       </c>
       <c r="E74" s="6">
-        <v>280149</v>
+        <v>176534</v>
       </c>
       <c r="F74">
         <v>7200</v>
@@ -2484,16 +2501,16 @@
         <v>73</v>
       </c>
       <c r="B75" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C75" s="6">
         <v>28800</v>
       </c>
       <c r="D75">
-        <v>82800</v>
+        <v>79200</v>
       </c>
       <c r="E75" s="6">
-        <v>216456</v>
+        <v>280149</v>
       </c>
       <c r="F75">
         <v>7200</v>
@@ -2504,16 +2521,16 @@
         <v>74</v>
       </c>
       <c r="B76" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C76" s="6">
-        <v>27000</v>
+        <v>28800</v>
       </c>
       <c r="D76">
-        <v>77400</v>
+        <v>82800</v>
       </c>
       <c r="E76" s="6">
-        <v>113922</v>
+        <v>216456</v>
       </c>
       <c r="F76">
         <v>7200</v>
@@ -2524,16 +2541,16 @@
         <v>75</v>
       </c>
       <c r="B77" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C77" s="6">
-        <v>28800</v>
+        <v>27000</v>
       </c>
       <c r="D77">
-        <v>79200</v>
+        <v>77400</v>
       </c>
       <c r="E77" s="6">
-        <v>236440</v>
+        <v>113922</v>
       </c>
       <c r="F77">
         <v>7200</v>
@@ -2544,16 +2561,16 @@
         <v>76</v>
       </c>
       <c r="B78" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C78" s="6">
-        <v>25200</v>
+        <v>28800</v>
       </c>
       <c r="D78">
         <v>79200</v>
       </c>
       <c r="E78" s="6">
-        <v>211451</v>
+        <v>236440</v>
       </c>
       <c r="F78">
         <v>7200</v>
@@ -2564,16 +2581,16 @@
         <v>77</v>
       </c>
       <c r="B79" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C79" s="6">
-        <v>39600</v>
+        <v>25200</v>
       </c>
       <c r="D79">
-        <v>77400</v>
+        <v>79200</v>
       </c>
       <c r="E79" s="6">
-        <v>154162</v>
+        <v>211451</v>
       </c>
       <c r="F79">
         <v>7200</v>
@@ -2584,16 +2601,16 @@
         <v>78</v>
       </c>
       <c r="B80" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C80" s="6">
-        <v>27000</v>
+        <v>39600</v>
       </c>
       <c r="D80">
-        <v>79200</v>
+        <v>77400</v>
       </c>
       <c r="E80" s="6">
-        <v>173799</v>
+        <v>154162</v>
       </c>
       <c r="F80">
         <v>7200</v>
@@ -2604,16 +2621,16 @@
         <v>79</v>
       </c>
       <c r="B81" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C81" s="6">
-        <v>32400</v>
+        <v>27000</v>
       </c>
       <c r="D81">
         <v>79200</v>
       </c>
       <c r="E81" s="6">
-        <v>122195</v>
+        <v>173799</v>
       </c>
       <c r="F81">
         <v>7200</v>
@@ -2624,7 +2641,7 @@
         <v>80</v>
       </c>
       <c r="B82" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C82" s="6">
         <v>32400</v>
@@ -2633,7 +2650,7 @@
         <v>79200</v>
       </c>
       <c r="E82" s="6">
-        <v>231609</v>
+        <v>122195</v>
       </c>
       <c r="F82">
         <v>7200</v>
@@ -2644,16 +2661,16 @@
         <v>81</v>
       </c>
       <c r="B83" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C83" s="6">
-        <v>28800</v>
+        <v>32400</v>
       </c>
       <c r="D83">
-        <v>75600</v>
+        <v>79200</v>
       </c>
       <c r="E83" s="6">
-        <v>216912</v>
+        <v>231609</v>
       </c>
       <c r="F83">
         <v>7200</v>
@@ -2664,16 +2681,16 @@
         <v>82</v>
       </c>
       <c r="B84" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C84" s="6">
-        <v>32400</v>
+        <v>28800</v>
       </c>
       <c r="D84">
-        <v>79200</v>
+        <v>75600</v>
       </c>
       <c r="E84" s="6">
-        <v>235074</v>
+        <v>216912</v>
       </c>
       <c r="F84">
         <v>7200</v>
@@ -2684,16 +2701,16 @@
         <v>83</v>
       </c>
       <c r="B85" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C85" s="6">
-        <v>28800</v>
+        <v>32400</v>
       </c>
       <c r="D85">
         <v>79200</v>
       </c>
       <c r="E85" s="6">
-        <v>171829</v>
+        <v>235074</v>
       </c>
       <c r="F85">
         <v>7200</v>
@@ -2704,7 +2721,7 @@
         <v>84</v>
       </c>
       <c r="B86" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C86" s="6">
         <v>28800</v>
@@ -2713,7 +2730,7 @@
         <v>79200</v>
       </c>
       <c r="E86" s="6">
-        <v>223353</v>
+        <v>171829</v>
       </c>
       <c r="F86">
         <v>7200</v>
@@ -2724,7 +2741,7 @@
         <v>85</v>
       </c>
       <c r="B87" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C87" s="6">
         <v>28800</v>
@@ -2733,7 +2750,7 @@
         <v>79200</v>
       </c>
       <c r="E87" s="6">
-        <v>121675</v>
+        <v>223353</v>
       </c>
       <c r="F87">
         <v>7200</v>
@@ -2744,16 +2761,16 @@
         <v>86</v>
       </c>
       <c r="B88" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C88" s="6">
         <v>28800</v>
       </c>
       <c r="D88">
-        <v>75600</v>
+        <v>79200</v>
       </c>
       <c r="E88" s="6">
-        <v>134040</v>
+        <v>121675</v>
       </c>
       <c r="F88">
         <v>7200</v>
@@ -2764,16 +2781,16 @@
         <v>87</v>
       </c>
       <c r="B89" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C89" s="6">
-        <v>25200</v>
+        <v>28800</v>
       </c>
       <c r="D89">
-        <v>61200</v>
+        <v>75600</v>
       </c>
       <c r="E89" s="6">
-        <v>162290</v>
+        <v>134040</v>
       </c>
       <c r="F89">
         <v>7200</v>
@@ -2784,16 +2801,16 @@
         <v>88</v>
       </c>
       <c r="B90" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C90" s="6">
-        <v>28800</v>
+        <v>25200</v>
       </c>
       <c r="D90">
-        <v>75600</v>
+        <v>61200</v>
       </c>
       <c r="E90" s="6">
-        <v>291734</v>
+        <v>162290</v>
       </c>
       <c r="F90">
         <v>7200</v>
@@ -2804,16 +2821,16 @@
         <v>89</v>
       </c>
       <c r="B91" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C91" s="6">
-        <v>37800</v>
+        <v>28800</v>
       </c>
       <c r="D91">
-        <v>45000</v>
+        <v>75600</v>
       </c>
       <c r="E91" s="6">
-        <v>148838</v>
+        <v>291734</v>
       </c>
       <c r="F91">
         <v>7200</v>
@@ -2824,16 +2841,16 @@
         <v>90</v>
       </c>
       <c r="B92" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C92" s="6">
-        <v>28800</v>
+        <v>37800</v>
       </c>
       <c r="D92">
-        <v>75600</v>
+        <v>45000</v>
       </c>
       <c r="E92" s="6">
-        <v>195424</v>
+        <v>148838</v>
       </c>
       <c r="F92">
         <v>7200</v>
@@ -2844,16 +2861,16 @@
         <v>91</v>
       </c>
       <c r="B93" t="s">
-        <v>96</v>
-      </c>
-      <c r="C93" s="7">
-        <v>30600</v>
-      </c>
-      <c r="D93" s="3">
-        <v>41400</v>
+        <v>95</v>
+      </c>
+      <c r="C93" s="6">
+        <v>28800</v>
+      </c>
+      <c r="D93">
+        <v>75600</v>
       </c>
       <c r="E93" s="6">
-        <v>279040</v>
+        <v>195424</v>
       </c>
       <c r="F93">
         <v>7200</v>
@@ -2864,16 +2881,16 @@
         <v>92</v>
       </c>
       <c r="B94" t="s">
-        <v>97</v>
-      </c>
-      <c r="C94" s="6">
-        <v>25200</v>
-      </c>
-      <c r="D94">
-        <v>64800</v>
+        <v>96</v>
+      </c>
+      <c r="C94" s="7">
+        <v>30600</v>
+      </c>
+      <c r="D94" s="3">
+        <v>41400</v>
       </c>
       <c r="E94" s="6">
-        <v>149058</v>
+        <v>279040</v>
       </c>
       <c r="F94">
         <v>7200</v>
@@ -2884,16 +2901,16 @@
         <v>93</v>
       </c>
       <c r="B95" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C95" s="6">
         <v>25200</v>
       </c>
       <c r="D95">
-        <v>61200</v>
+        <v>64800</v>
       </c>
       <c r="E95" s="6">
-        <v>251955</v>
+        <v>149058</v>
       </c>
       <c r="F95">
         <v>7200</v>
@@ -2904,16 +2921,16 @@
         <v>94</v>
       </c>
       <c r="B96" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C96" s="6">
         <v>25200</v>
       </c>
       <c r="D96">
-        <v>77400</v>
+        <v>61200</v>
       </c>
       <c r="E96" s="6">
-        <v>282070</v>
+        <v>251955</v>
       </c>
       <c r="F96">
         <v>7200</v>
@@ -2924,16 +2941,16 @@
         <v>95</v>
       </c>
       <c r="B97" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C97" s="6">
-        <v>28800</v>
+        <v>25200</v>
       </c>
       <c r="D97">
-        <v>75600</v>
+        <v>77400</v>
       </c>
       <c r="E97" s="6">
-        <v>155925</v>
+        <v>282070</v>
       </c>
       <c r="F97">
         <v>7200</v>
@@ -2944,16 +2961,16 @@
         <v>96</v>
       </c>
       <c r="B98" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C98" s="6">
-        <v>30600</v>
+        <v>28800</v>
       </c>
       <c r="D98">
-        <v>77400</v>
+        <v>75600</v>
       </c>
       <c r="E98" s="6">
-        <v>102141</v>
+        <v>155925</v>
       </c>
       <c r="F98">
         <v>7200</v>
@@ -2964,16 +2981,16 @@
         <v>97</v>
       </c>
       <c r="B99" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C99" s="6">
-        <v>27000</v>
+        <v>30600</v>
       </c>
       <c r="D99">
-        <v>61200</v>
+        <v>77400</v>
       </c>
       <c r="E99" s="6">
-        <v>246509</v>
+        <v>102141</v>
       </c>
       <c r="F99">
         <v>7200</v>
@@ -2984,16 +3001,16 @@
         <v>98</v>
       </c>
       <c r="B100" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C100" s="6">
-        <v>34200</v>
+        <v>27000</v>
       </c>
       <c r="D100">
-        <v>75600</v>
+        <v>61200</v>
       </c>
       <c r="E100" s="6">
-        <v>249444</v>
+        <v>246509</v>
       </c>
       <c r="F100">
         <v>7200</v>
@@ -3004,16 +3021,16 @@
         <v>99</v>
       </c>
       <c r="B101" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C101" s="6">
-        <v>28800</v>
+        <v>34200</v>
       </c>
       <c r="D101">
-        <v>79200</v>
+        <v>75600</v>
       </c>
       <c r="E101" s="6">
-        <v>181346</v>
+        <v>249444</v>
       </c>
       <c r="F101">
         <v>7200</v>
@@ -3024,7 +3041,7 @@
         <v>100</v>
       </c>
       <c r="B102" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C102" s="6">
         <v>28800</v>
@@ -3033,7 +3050,7 @@
         <v>79200</v>
       </c>
       <c r="E102" s="6">
-        <v>188022</v>
+        <v>181346</v>
       </c>
       <c r="F102">
         <v>7200</v>
@@ -3044,7 +3061,7 @@
         <v>101</v>
       </c>
       <c r="B103" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C103" s="6">
         <v>28800</v>
@@ -3053,7 +3070,7 @@
         <v>79200</v>
       </c>
       <c r="E103" s="6">
-        <v>287654</v>
+        <v>188022</v>
       </c>
       <c r="F103">
         <v>7200</v>
@@ -3064,16 +3081,16 @@
         <v>102</v>
       </c>
       <c r="B104" t="s">
-        <v>107</v>
-      </c>
-      <c r="C104" s="8">
-        <v>0</v>
-      </c>
-      <c r="D104" s="8">
-        <v>86400</v>
+        <v>106</v>
+      </c>
+      <c r="C104" s="6">
+        <v>28800</v>
+      </c>
+      <c r="D104">
+        <v>79200</v>
       </c>
       <c r="E104" s="6">
-        <v>126070</v>
+        <v>287654</v>
       </c>
       <c r="F104">
         <v>7200</v>
@@ -3084,16 +3101,16 @@
         <v>103</v>
       </c>
       <c r="B105" t="s">
-        <v>108</v>
-      </c>
-      <c r="C105" s="6">
-        <v>36000</v>
-      </c>
-      <c r="D105">
-        <v>79200</v>
+        <v>107</v>
+      </c>
+      <c r="C105" s="8">
+        <v>0</v>
+      </c>
+      <c r="D105" s="8">
+        <v>86400</v>
       </c>
       <c r="E105" s="6">
-        <v>277462</v>
+        <v>126070</v>
       </c>
       <c r="F105">
         <v>7200</v>
@@ -3104,16 +3121,16 @@
         <v>104</v>
       </c>
       <c r="B106" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C106" s="6">
-        <v>25200</v>
+        <v>36000</v>
       </c>
       <c r="D106">
         <v>79200</v>
       </c>
       <c r="E106" s="6">
-        <v>295181</v>
+        <v>277462</v>
       </c>
       <c r="F106">
         <v>7200</v>
@@ -3124,16 +3141,16 @@
         <v>105</v>
       </c>
       <c r="B107" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C107" s="6">
-        <v>32400</v>
+        <v>25200</v>
       </c>
       <c r="D107">
-        <v>75600</v>
+        <v>79200</v>
       </c>
       <c r="E107" s="6">
-        <v>241705</v>
+        <v>295181</v>
       </c>
       <c r="F107">
         <v>7200</v>
@@ -3144,16 +3161,16 @@
         <v>106</v>
       </c>
       <c r="B108" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C108" s="6">
-        <v>68400</v>
-      </c>
-      <c r="D108" s="4">
-        <v>97200</v>
+        <v>32400</v>
+      </c>
+      <c r="D108">
+        <v>75600</v>
       </c>
       <c r="E108" s="6">
-        <v>168526</v>
+        <v>241705</v>
       </c>
       <c r="F108">
         <v>7200</v>
@@ -3164,16 +3181,16 @@
         <v>107</v>
       </c>
       <c r="B109" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C109" s="6">
-        <v>28800</v>
-      </c>
-      <c r="D109">
-        <v>77400</v>
+        <v>68400</v>
+      </c>
+      <c r="D109" s="4">
+        <v>97200</v>
       </c>
       <c r="E109" s="6">
-        <v>242233</v>
+        <v>168526</v>
       </c>
       <c r="F109">
         <v>7200</v>
@@ -3184,16 +3201,16 @@
         <v>108</v>
       </c>
       <c r="B110" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C110" s="6">
-        <v>36000</v>
+        <v>28800</v>
       </c>
       <c r="D110">
-        <v>75600</v>
+        <v>77400</v>
       </c>
       <c r="E110" s="6">
-        <v>169997</v>
+        <v>242233</v>
       </c>
       <c r="F110">
         <v>7200</v>
@@ -3204,16 +3221,16 @@
         <v>109</v>
       </c>
       <c r="B111" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C111" s="6">
-        <v>28800</v>
+        <v>36000</v>
       </c>
       <c r="D111">
-        <v>79200</v>
+        <v>75600</v>
       </c>
       <c r="E111" s="6">
-        <v>161010</v>
+        <v>169997</v>
       </c>
       <c r="F111">
         <v>7200</v>
@@ -3224,16 +3241,16 @@
         <v>110</v>
       </c>
       <c r="B112" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C112" s="6">
-        <v>36000</v>
+        <v>28800</v>
       </c>
       <c r="D112">
         <v>79200</v>
       </c>
       <c r="E112" s="6">
-        <v>125417</v>
+        <v>161010</v>
       </c>
       <c r="F112">
         <v>7200</v>
@@ -3244,16 +3261,16 @@
         <v>111</v>
       </c>
       <c r="B113" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C113" s="6">
-        <v>25200</v>
+        <v>36000</v>
       </c>
       <c r="D113">
-        <v>43200</v>
+        <v>79200</v>
       </c>
       <c r="E113" s="6">
-        <v>183369</v>
+        <v>125417</v>
       </c>
       <c r="F113">
         <v>7200</v>
@@ -3264,16 +3281,16 @@
         <v>112</v>
       </c>
       <c r="B114" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C114" s="6">
         <v>25200</v>
       </c>
       <c r="D114">
-        <v>75600</v>
+        <v>43200</v>
       </c>
       <c r="E114" s="6">
-        <v>293671</v>
+        <v>183369</v>
       </c>
       <c r="F114">
         <v>7200</v>
@@ -3284,16 +3301,16 @@
         <v>113</v>
       </c>
       <c r="B115" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C115" s="6">
-        <v>32400</v>
+        <v>25200</v>
       </c>
       <c r="D115">
-        <v>77400</v>
+        <v>75600</v>
       </c>
       <c r="E115" s="6">
-        <v>292574</v>
+        <v>293671</v>
       </c>
       <c r="F115">
         <v>7200</v>
@@ -3304,16 +3321,16 @@
         <v>114</v>
       </c>
       <c r="B116" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C116" s="6">
-        <v>28800</v>
+        <v>32400</v>
       </c>
       <c r="D116">
-        <v>75600</v>
+        <v>77400</v>
       </c>
       <c r="E116" s="6">
-        <v>251917</v>
+        <v>292574</v>
       </c>
       <c r="F116">
         <v>7200</v>
@@ -3324,16 +3341,16 @@
         <v>115</v>
       </c>
       <c r="B117" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C117" s="6">
-        <v>27000</v>
+        <v>28800</v>
       </c>
       <c r="D117">
-        <v>61200</v>
+        <v>75600</v>
       </c>
       <c r="E117" s="6">
-        <v>135538</v>
+        <v>251917</v>
       </c>
       <c r="F117">
         <v>7200</v>
@@ -3344,16 +3361,16 @@
         <v>116</v>
       </c>
       <c r="B118" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C118" s="6">
         <v>27000</v>
       </c>
       <c r="D118">
-        <v>75600</v>
+        <v>61200</v>
       </c>
       <c r="E118" s="6">
-        <v>281034</v>
+        <v>135538</v>
       </c>
       <c r="F118">
         <v>7200</v>
@@ -3364,16 +3381,16 @@
         <v>117</v>
       </c>
       <c r="B119" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C119" s="6">
-        <v>25200</v>
+        <v>27000</v>
       </c>
       <c r="D119">
         <v>75600</v>
       </c>
       <c r="E119" s="6">
-        <v>243086</v>
+        <v>281034</v>
       </c>
       <c r="F119">
         <v>7200</v>
@@ -3384,16 +3401,16 @@
         <v>118</v>
       </c>
       <c r="B120" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C120" s="6">
-        <v>28800</v>
+        <v>25200</v>
       </c>
       <c r="D120">
-        <v>79200</v>
+        <v>75600</v>
       </c>
       <c r="E120" s="6">
-        <v>293296</v>
+        <v>243086</v>
       </c>
       <c r="F120">
         <v>7200</v>
@@ -3404,7 +3421,7 @@
         <v>119</v>
       </c>
       <c r="B121" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C121" s="6">
         <v>28800</v>
@@ -3413,7 +3430,7 @@
         <v>79200</v>
       </c>
       <c r="E121" s="6">
-        <v>247136</v>
+        <v>293296</v>
       </c>
       <c r="F121">
         <v>7200</v>
@@ -3424,16 +3441,16 @@
         <v>120</v>
       </c>
       <c r="B122" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C122" s="6">
         <v>28800</v>
       </c>
       <c r="D122">
-        <v>81000</v>
+        <v>79200</v>
       </c>
       <c r="E122" s="6">
-        <v>133993</v>
+        <v>247136</v>
       </c>
       <c r="F122">
         <v>7200</v>
@@ -3444,16 +3461,16 @@
         <v>121</v>
       </c>
       <c r="B123" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C123" s="6">
         <v>28800</v>
       </c>
       <c r="D123">
-        <v>79200</v>
+        <v>81000</v>
       </c>
       <c r="E123" s="6">
-        <v>208426</v>
+        <v>133993</v>
       </c>
       <c r="F123">
         <v>7200</v>
@@ -3464,16 +3481,16 @@
         <v>122</v>
       </c>
       <c r="B124" t="s">
-        <v>127</v>
-      </c>
-      <c r="C124" s="8">
-        <v>0</v>
-      </c>
-      <c r="D124" s="8">
-        <v>86400</v>
+        <v>126</v>
+      </c>
+      <c r="C124" s="6">
+        <v>28800</v>
+      </c>
+      <c r="D124">
+        <v>79200</v>
       </c>
       <c r="E124" s="6">
-        <v>199011</v>
+        <v>208426</v>
       </c>
       <c r="F124">
         <v>7200</v>
@@ -3484,16 +3501,16 @@
         <v>123</v>
       </c>
       <c r="B125" t="s">
-        <v>128</v>
-      </c>
-      <c r="C125" s="6">
-        <v>25200</v>
-      </c>
-      <c r="D125">
-        <v>75600</v>
+        <v>127</v>
+      </c>
+      <c r="C125" s="8">
+        <v>0</v>
+      </c>
+      <c r="D125" s="8">
+        <v>86400</v>
       </c>
       <c r="E125" s="6">
-        <v>210140</v>
+        <v>199011</v>
       </c>
       <c r="F125">
         <v>7200</v>
@@ -3504,16 +3521,16 @@
         <v>124</v>
       </c>
       <c r="B126" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C126" s="6">
-        <v>28800</v>
+        <v>25200</v>
       </c>
       <c r="D126">
-        <v>64800</v>
+        <v>75600</v>
       </c>
       <c r="E126" s="6">
-        <v>246008</v>
+        <v>210140</v>
       </c>
       <c r="F126">
         <v>7200</v>
@@ -3524,16 +3541,16 @@
         <v>125</v>
       </c>
       <c r="B127" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C127" s="6">
-        <v>36000</v>
+        <v>28800</v>
       </c>
       <c r="D127">
-        <v>79200</v>
+        <v>64800</v>
       </c>
       <c r="E127" s="6">
-        <v>118173</v>
+        <v>246008</v>
       </c>
       <c r="F127">
         <v>7200</v>
@@ -3544,16 +3561,16 @@
         <v>126</v>
       </c>
       <c r="B128" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C128" s="6">
-        <v>34200</v>
+        <v>36000</v>
       </c>
       <c r="D128">
         <v>79200</v>
       </c>
       <c r="E128" s="6">
-        <v>266817</v>
+        <v>118173</v>
       </c>
       <c r="F128">
         <v>7200</v>
@@ -3564,7 +3581,7 @@
         <v>127</v>
       </c>
       <c r="B129" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C129" s="6">
         <v>34200</v>
@@ -3573,7 +3590,7 @@
         <v>79200</v>
       </c>
       <c r="E129" s="6">
-        <v>153946</v>
+        <v>266817</v>
       </c>
       <c r="F129">
         <v>7200</v>
@@ -3584,16 +3601,16 @@
         <v>128</v>
       </c>
       <c r="B130" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C130" s="6">
-        <v>28800</v>
+        <v>34200</v>
       </c>
       <c r="D130">
         <v>79200</v>
       </c>
       <c r="E130" s="6">
-        <v>280189</v>
+        <v>153946</v>
       </c>
       <c r="F130">
         <v>7200</v>
@@ -3604,16 +3621,16 @@
         <v>129</v>
       </c>
       <c r="B131" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C131" s="6">
-        <v>25200</v>
+        <v>28800</v>
       </c>
       <c r="D131">
-        <v>61200</v>
+        <v>79200</v>
       </c>
       <c r="E131" s="6">
-        <v>110079</v>
+        <v>280189</v>
       </c>
       <c r="F131">
         <v>7200</v>
@@ -3624,16 +3641,16 @@
         <v>130</v>
       </c>
       <c r="B132" t="s">
-        <v>135</v>
-      </c>
-      <c r="C132" s="7">
-        <v>28800</v>
-      </c>
-      <c r="D132" s="3">
-        <v>39600</v>
+        <v>134</v>
+      </c>
+      <c r="C132" s="6">
+        <v>25200</v>
+      </c>
+      <c r="D132">
+        <v>61200</v>
       </c>
       <c r="E132" s="6">
-        <v>277642</v>
+        <v>110079</v>
       </c>
       <c r="F132">
         <v>7200</v>
@@ -3644,16 +3661,16 @@
         <v>131</v>
       </c>
       <c r="B133" t="s">
-        <v>136</v>
-      </c>
-      <c r="C133" s="6">
-        <v>32400</v>
-      </c>
-      <c r="D133">
-        <v>61200</v>
+        <v>135</v>
+      </c>
+      <c r="C133" s="7">
+        <v>28800</v>
+      </c>
+      <c r="D133" s="3">
+        <v>39600</v>
       </c>
       <c r="E133" s="6">
-        <v>231474</v>
+        <v>277642</v>
       </c>
       <c r="F133">
         <v>7200</v>
@@ -3664,16 +3681,16 @@
         <v>132</v>
       </c>
       <c r="B134" t="s">
-        <v>137</v>
-      </c>
-      <c r="C134" s="8">
-        <v>0</v>
-      </c>
-      <c r="D134" s="8">
-        <v>86400</v>
+        <v>136</v>
+      </c>
+      <c r="C134" s="6">
+        <v>32400</v>
+      </c>
+      <c r="D134">
+        <v>61200</v>
       </c>
       <c r="E134" s="6">
-        <v>174920</v>
+        <v>231474</v>
       </c>
       <c r="F134">
         <v>7200</v>
@@ -3684,16 +3701,16 @@
         <v>133</v>
       </c>
       <c r="B135" t="s">
-        <v>138</v>
-      </c>
-      <c r="C135" s="6">
-        <v>21600</v>
-      </c>
-      <c r="D135">
-        <v>79200</v>
+        <v>137</v>
+      </c>
+      <c r="C135" s="8">
+        <v>0</v>
+      </c>
+      <c r="D135" s="8">
+        <v>86400</v>
       </c>
       <c r="E135" s="6">
-        <v>142842</v>
+        <v>174920</v>
       </c>
       <c r="F135">
         <v>7200</v>
@@ -3704,16 +3721,16 @@
         <v>134</v>
       </c>
       <c r="B136" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C136" s="6">
-        <v>28800</v>
+        <v>21600</v>
       </c>
       <c r="D136">
         <v>79200</v>
       </c>
       <c r="E136" s="6">
-        <v>122094</v>
+        <v>142842</v>
       </c>
       <c r="F136">
         <v>7200</v>
@@ -3724,16 +3741,16 @@
         <v>135</v>
       </c>
       <c r="B137" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C137" s="6">
-        <v>32400</v>
+        <v>28800</v>
       </c>
       <c r="D137">
-        <v>61200</v>
+        <v>79200</v>
       </c>
       <c r="E137" s="6">
-        <v>255775</v>
+        <v>122094</v>
       </c>
       <c r="F137">
         <v>7200</v>
@@ -3744,16 +3761,16 @@
         <v>136</v>
       </c>
       <c r="B138" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C138" s="6">
-        <v>28800</v>
+        <v>32400</v>
       </c>
       <c r="D138">
-        <v>79200</v>
+        <v>61200</v>
       </c>
       <c r="E138" s="6">
-        <v>158666</v>
+        <v>255775</v>
       </c>
       <c r="F138">
         <v>7200</v>
@@ -3764,16 +3781,16 @@
         <v>137</v>
       </c>
       <c r="B139" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C139" s="6">
-        <v>30600</v>
+        <v>28800</v>
       </c>
       <c r="D139">
-        <v>68400</v>
+        <v>79200</v>
       </c>
       <c r="E139" s="6">
-        <v>145252</v>
+        <v>158666</v>
       </c>
       <c r="F139">
         <v>7200</v>
@@ -3784,16 +3801,16 @@
         <v>138</v>
       </c>
       <c r="B140" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C140" s="6">
-        <v>25200</v>
+        <v>30600</v>
       </c>
       <c r="D140">
-        <v>79200</v>
+        <v>68400</v>
       </c>
       <c r="E140" s="6">
-        <v>113950</v>
+        <v>145252</v>
       </c>
       <c r="F140">
         <v>7200</v>
@@ -3804,16 +3821,16 @@
         <v>139</v>
       </c>
       <c r="B141" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C141" s="6">
-        <v>27000</v>
+        <v>25200</v>
       </c>
       <c r="D141">
-        <v>64800</v>
+        <v>79200</v>
       </c>
       <c r="E141" s="6">
-        <v>131914</v>
+        <v>113950</v>
       </c>
       <c r="F141">
         <v>7200</v>
@@ -3824,16 +3841,16 @@
         <v>140</v>
       </c>
       <c r="B142" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C142" s="6">
         <v>27000</v>
       </c>
       <c r="D142">
-        <v>79200</v>
+        <v>64800</v>
       </c>
       <c r="E142" s="6">
-        <v>117409</v>
+        <v>131914</v>
       </c>
       <c r="F142">
         <v>7200</v>
@@ -3844,16 +3861,16 @@
         <v>141</v>
       </c>
       <c r="B143" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C143" s="6">
-        <v>32400</v>
+        <v>27000</v>
       </c>
       <c r="D143">
         <v>79200</v>
       </c>
       <c r="E143" s="6">
-        <v>234001</v>
+        <v>117409</v>
       </c>
       <c r="F143">
         <v>7200</v>
@@ -3864,16 +3881,16 @@
         <v>142</v>
       </c>
       <c r="B144" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C144" s="6">
-        <v>34200</v>
+        <v>32400</v>
       </c>
       <c r="D144">
-        <v>72000</v>
+        <v>79200</v>
       </c>
       <c r="E144" s="6">
-        <v>299031</v>
+        <v>234001</v>
       </c>
       <c r="F144">
         <v>7200</v>
@@ -3884,16 +3901,16 @@
         <v>143</v>
       </c>
       <c r="B145" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C145" s="6">
-        <v>36000</v>
+        <v>34200</v>
       </c>
       <c r="D145">
-        <v>79200</v>
+        <v>72000</v>
       </c>
       <c r="E145" s="6">
-        <v>260391</v>
+        <v>299031</v>
       </c>
       <c r="F145">
         <v>7200</v>
@@ -3904,16 +3921,16 @@
         <v>144</v>
       </c>
       <c r="B146" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C146" s="6">
-        <v>30600</v>
+        <v>36000</v>
       </c>
       <c r="D146">
-        <v>61200</v>
+        <v>79200</v>
       </c>
       <c r="E146" s="6">
-        <v>124759</v>
+        <v>260391</v>
       </c>
       <c r="F146">
         <v>7200</v>
@@ -3924,16 +3941,16 @@
         <v>145</v>
       </c>
       <c r="B147" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C147" s="6">
-        <v>25200</v>
+        <v>30600</v>
       </c>
       <c r="D147">
-        <v>68400</v>
+        <v>61200</v>
       </c>
       <c r="E147" s="6">
-        <v>283782</v>
+        <v>124759</v>
       </c>
       <c r="F147">
         <v>7200</v>
@@ -3944,16 +3961,16 @@
         <v>146</v>
       </c>
       <c r="B148" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C148" s="6">
-        <v>32400</v>
+        <v>25200</v>
       </c>
       <c r="D148">
-        <v>72000</v>
+        <v>68400</v>
       </c>
       <c r="E148" s="6">
-        <v>118803</v>
+        <v>283782</v>
       </c>
       <c r="F148">
         <v>7200</v>
@@ -3964,16 +3981,16 @@
         <v>147</v>
       </c>
       <c r="B149" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C149" s="6">
-        <v>21600</v>
+        <v>32400</v>
       </c>
       <c r="D149">
-        <v>79200</v>
-      </c>
-      <c r="E149" s="9">
-        <v>500000</v>
+        <v>72000</v>
+      </c>
+      <c r="E149" s="6">
+        <v>118803</v>
       </c>
       <c r="F149">
         <v>7200</v>
@@ -3984,16 +4001,16 @@
         <v>148</v>
       </c>
       <c r="B150" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C150" s="6">
-        <v>25200</v>
+        <v>21600</v>
       </c>
       <c r="D150">
         <v>79200</v>
       </c>
-      <c r="E150" s="6">
-        <v>50000</v>
+      <c r="E150" s="9">
+        <v>500000</v>
       </c>
       <c r="F150">
         <v>7200</v>
@@ -4004,7 +4021,7 @@
         <v>149</v>
       </c>
       <c r="B151" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C151" s="6">
         <v>25200</v>
@@ -4013,7 +4030,7 @@
         <v>79200</v>
       </c>
       <c r="E151" s="6">
-        <v>30000</v>
+        <v>50000</v>
       </c>
       <c r="F151">
         <v>7200</v>
@@ -4024,16 +4041,16 @@
         <v>150</v>
       </c>
       <c r="B152" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C152" s="6">
-        <v>32400</v>
+        <v>25200</v>
       </c>
       <c r="D152">
-        <v>77400</v>
+        <v>79200</v>
       </c>
       <c r="E152" s="6">
-        <v>500000</v>
+        <v>30000</v>
       </c>
       <c r="F152">
         <v>7200</v>
@@ -4044,16 +4061,16 @@
         <v>151</v>
       </c>
       <c r="B153" t="s">
-        <v>156</v>
-      </c>
-      <c r="C153" s="8">
-        <v>0</v>
-      </c>
-      <c r="D153" s="8">
-        <v>86400</v>
+        <v>155</v>
+      </c>
+      <c r="C153" s="6">
+        <v>32400</v>
+      </c>
+      <c r="D153">
+        <v>77400</v>
       </c>
       <c r="E153" s="6">
-        <v>300000</v>
+        <v>500000</v>
       </c>
       <c r="F153">
         <v>7200</v>
@@ -4064,16 +4081,16 @@
         <v>152</v>
       </c>
       <c r="B154" t="s">
-        <v>157</v>
-      </c>
-      <c r="C154" s="6">
-        <v>16200</v>
-      </c>
-      <c r="D154">
-        <v>37800</v>
+        <v>156</v>
+      </c>
+      <c r="C154" s="8">
+        <v>0</v>
+      </c>
+      <c r="D154" s="8">
+        <v>86400</v>
       </c>
       <c r="E154" s="6">
-        <v>1000000</v>
+        <v>300000</v>
       </c>
       <c r="F154">
         <v>7200</v>
@@ -4084,16 +4101,16 @@
         <v>153</v>
       </c>
       <c r="B155" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C155" s="6">
-        <v>28800</v>
+        <v>16200</v>
       </c>
       <c r="D155">
-        <v>79200</v>
+        <v>37800</v>
       </c>
       <c r="E155" s="6">
-        <v>136364</v>
+        <v>1000000</v>
       </c>
       <c r="F155">
         <v>7200</v>
@@ -4104,16 +4121,16 @@
         <v>154</v>
       </c>
       <c r="B156" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C156" s="6">
-        <v>32400</v>
+        <v>28800</v>
       </c>
       <c r="D156">
         <v>79200</v>
       </c>
       <c r="E156" s="6">
-        <v>150000</v>
+        <v>136364</v>
       </c>
       <c r="F156">
         <v>7200</v>
@@ -4124,16 +4141,16 @@
         <v>155</v>
       </c>
       <c r="B157" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C157" s="6">
-        <v>41400</v>
+        <v>32400</v>
       </c>
       <c r="D157">
-        <v>82800</v>
+        <v>79200</v>
       </c>
       <c r="E157" s="6">
-        <v>400000</v>
+        <v>150000</v>
       </c>
       <c r="F157">
         <v>7200</v>
@@ -4144,16 +4161,16 @@
         <v>156</v>
       </c>
       <c r="B158" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C158" s="6">
-        <v>36000</v>
+        <v>41400</v>
       </c>
       <c r="D158">
         <v>82800</v>
       </c>
       <c r="E158" s="6">
-        <v>350000</v>
+        <v>400000</v>
       </c>
       <c r="F158">
         <v>7200</v>
@@ -4164,16 +4181,16 @@
         <v>157</v>
       </c>
       <c r="B159" t="s">
-        <v>162</v>
-      </c>
-      <c r="C159" s="8">
-        <v>0</v>
-      </c>
-      <c r="D159" s="8">
-        <v>86400</v>
+        <v>161</v>
+      </c>
+      <c r="C159" s="6">
+        <v>36000</v>
+      </c>
+      <c r="D159">
+        <v>82800</v>
       </c>
       <c r="E159" s="6">
-        <v>227273</v>
+        <v>350000</v>
       </c>
       <c r="F159">
         <v>7200</v>
@@ -4184,7 +4201,7 @@
         <v>158</v>
       </c>
       <c r="B160" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C160" s="8">
         <v>0</v>
@@ -4193,7 +4210,7 @@
         <v>86400</v>
       </c>
       <c r="E160" s="6">
-        <v>150000</v>
+        <v>227273</v>
       </c>
       <c r="F160">
         <v>7200</v>
@@ -4204,16 +4221,16 @@
         <v>159</v>
       </c>
       <c r="B161" t="s">
-        <v>164</v>
-      </c>
-      <c r="C161" s="6">
-        <v>28800</v>
-      </c>
-      <c r="D161">
-        <v>84600</v>
+        <v>163</v>
+      </c>
+      <c r="C161" s="8">
+        <v>0</v>
+      </c>
+      <c r="D161" s="8">
+        <v>86400</v>
       </c>
       <c r="E161" s="6">
-        <v>400000</v>
+        <v>150000</v>
       </c>
       <c r="F161">
         <v>7200</v>
@@ -4224,16 +4241,16 @@
         <v>160</v>
       </c>
       <c r="B162" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C162" s="6">
         <v>28800</v>
       </c>
       <c r="D162">
-        <v>79200</v>
+        <v>84600</v>
       </c>
       <c r="E162" s="6">
-        <v>340909</v>
+        <v>400000</v>
       </c>
       <c r="F162">
         <v>7200</v>
@@ -4244,16 +4261,16 @@
         <v>161</v>
       </c>
       <c r="B163" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C163" s="6">
-        <v>25200</v>
+        <v>28800</v>
       </c>
       <c r="D163">
-        <v>77400</v>
+        <v>79200</v>
       </c>
       <c r="E163" s="6">
-        <v>70000</v>
+        <v>340909</v>
       </c>
       <c r="F163">
         <v>7200</v>
@@ -4264,16 +4281,16 @@
         <v>162</v>
       </c>
       <c r="B164" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C164" s="6">
-        <v>32400</v>
+        <v>25200</v>
       </c>
       <c r="D164">
         <v>77400</v>
       </c>
       <c r="E164" s="6">
-        <v>340909</v>
+        <v>70000</v>
       </c>
       <c r="F164">
         <v>7200</v>
@@ -4284,16 +4301,16 @@
         <v>163</v>
       </c>
       <c r="B165" t="s">
-        <v>168</v>
-      </c>
-      <c r="C165" s="8">
-        <v>0</v>
-      </c>
-      <c r="D165" s="8">
-        <v>86400</v>
+        <v>167</v>
+      </c>
+      <c r="C165" s="6">
+        <v>32400</v>
+      </c>
+      <c r="D165">
+        <v>77400</v>
       </c>
       <c r="E165" s="6">
-        <v>400000</v>
+        <v>340909</v>
       </c>
       <c r="F165">
         <v>7200</v>
@@ -4304,16 +4321,16 @@
         <v>164</v>
       </c>
       <c r="B166" t="s">
-        <v>169</v>
-      </c>
-      <c r="C166" s="6">
-        <v>21600</v>
-      </c>
-      <c r="D166">
-        <v>81000</v>
+        <v>168</v>
+      </c>
+      <c r="C166" s="8">
+        <v>0</v>
+      </c>
+      <c r="D166" s="8">
+        <v>86400</v>
       </c>
       <c r="E166" s="6">
-        <v>454545</v>
+        <v>400000</v>
       </c>
       <c r="F166">
         <v>7200</v>
@@ -4324,16 +4341,16 @@
         <v>165</v>
       </c>
       <c r="B167" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C167" s="6">
         <v>21600</v>
       </c>
       <c r="D167">
-        <v>79200</v>
+        <v>81000</v>
       </c>
       <c r="E167" s="6">
-        <v>600000</v>
+        <v>454545</v>
       </c>
       <c r="F167">
         <v>7200</v>
@@ -4344,16 +4361,16 @@
         <v>166</v>
       </c>
       <c r="B168" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C168" s="6">
-        <v>30600</v>
+        <v>21600</v>
       </c>
       <c r="D168">
-        <v>75600</v>
+        <v>79200</v>
       </c>
       <c r="E168" s="6">
-        <v>500000</v>
+        <v>600000</v>
       </c>
       <c r="F168">
         <v>7200</v>
@@ -4364,16 +4381,16 @@
         <v>167</v>
       </c>
       <c r="B169" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C169" s="6">
-        <v>25200</v>
+        <v>30600</v>
       </c>
       <c r="D169">
-        <v>79200</v>
+        <v>75600</v>
       </c>
       <c r="E169" s="6">
-        <v>340909</v>
+        <v>500000</v>
       </c>
       <c r="F169">
         <v>7200</v>
@@ -4384,16 +4401,16 @@
         <v>168</v>
       </c>
       <c r="B170" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C170" s="6">
-        <v>39600</v>
+        <v>25200</v>
       </c>
       <c r="D170">
         <v>79200</v>
       </c>
       <c r="E170" s="6">
-        <v>800000</v>
+        <v>340909</v>
       </c>
       <c r="F170">
         <v>7200</v>
@@ -4404,16 +4421,16 @@
         <v>169</v>
       </c>
       <c r="B171" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C171" s="6">
-        <v>28800</v>
+        <v>39600</v>
       </c>
       <c r="D171">
-        <v>81000</v>
+        <v>79200</v>
       </c>
       <c r="E171" s="6">
-        <v>227273</v>
+        <v>800000</v>
       </c>
       <c r="F171">
         <v>7200</v>
@@ -4424,16 +4441,16 @@
         <v>170</v>
       </c>
       <c r="B172" t="s">
-        <v>175</v>
-      </c>
-      <c r="C172" s="7">
-        <v>36000</v>
-      </c>
-      <c r="D172" s="3">
-        <v>50400</v>
+        <v>174</v>
+      </c>
+      <c r="C172" s="6">
+        <v>28800</v>
+      </c>
+      <c r="D172">
+        <v>81000</v>
       </c>
       <c r="E172" s="6">
-        <v>500000</v>
+        <v>227273</v>
       </c>
       <c r="F172">
         <v>7200</v>
@@ -4444,16 +4461,16 @@
         <v>171</v>
       </c>
       <c r="B173" t="s">
-        <v>176</v>
-      </c>
-      <c r="C173" s="6">
-        <v>32400</v>
+        <v>175</v>
+      </c>
+      <c r="C173" s="7">
+        <v>36000</v>
       </c>
       <c r="D173" s="3">
-        <v>90000</v>
+        <v>50400</v>
       </c>
       <c r="E173" s="6">
-        <v>450000</v>
+        <v>500000</v>
       </c>
       <c r="F173">
         <v>7200</v>
@@ -4464,16 +4481,16 @@
         <v>172</v>
       </c>
       <c r="B174" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C174" s="6">
-        <v>36000</v>
-      </c>
-      <c r="D174">
-        <v>82800</v>
+        <v>32400</v>
+      </c>
+      <c r="D174" s="3">
+        <v>90000</v>
       </c>
       <c r="E174" s="6">
-        <v>300000</v>
+        <v>450000</v>
       </c>
       <c r="F174">
         <v>7200</v>
@@ -4484,13 +4501,13 @@
         <v>173</v>
       </c>
       <c r="B175" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C175" s="6">
-        <v>32400</v>
+        <v>36000</v>
       </c>
       <c r="D175">
-        <v>84600</v>
+        <v>82800</v>
       </c>
       <c r="E175" s="6">
         <v>300000</v>
@@ -4504,16 +4521,16 @@
         <v>174</v>
       </c>
       <c r="B176" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C176" s="6">
-        <v>36000</v>
+        <v>32400</v>
       </c>
       <c r="D176">
-        <v>82800</v>
+        <v>84600</v>
       </c>
       <c r="E176" s="6">
-        <v>340909</v>
+        <v>300000</v>
       </c>
       <c r="F176">
         <v>7200</v>
@@ -4524,16 +4541,16 @@
         <v>175</v>
       </c>
       <c r="B177" t="s">
-        <v>180</v>
-      </c>
-      <c r="C177" s="8">
-        <v>0</v>
-      </c>
-      <c r="D177" s="8">
-        <v>86400</v>
+        <v>179</v>
+      </c>
+      <c r="C177" s="6">
+        <v>36000</v>
+      </c>
+      <c r="D177">
+        <v>82800</v>
       </c>
       <c r="E177" s="6">
-        <v>350000</v>
+        <v>340909</v>
       </c>
       <c r="F177">
         <v>7200</v>
@@ -4544,16 +4561,16 @@
         <v>176</v>
       </c>
       <c r="B178" t="s">
-        <v>181</v>
-      </c>
-      <c r="C178" s="6">
-        <v>32400</v>
-      </c>
-      <c r="D178">
-        <v>82800</v>
+        <v>180</v>
+      </c>
+      <c r="C178" s="8">
+        <v>0</v>
+      </c>
+      <c r="D178" s="8">
+        <v>86400</v>
       </c>
       <c r="E178" s="6">
-        <v>454545</v>
+        <v>350000</v>
       </c>
       <c r="F178">
         <v>7200</v>
@@ -4564,16 +4581,16 @@
         <v>177</v>
       </c>
       <c r="B179" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C179" s="6">
-        <v>28800</v>
+        <v>32400</v>
       </c>
       <c r="D179">
-        <v>79200</v>
+        <v>82800</v>
       </c>
       <c r="E179" s="6">
-        <v>300000</v>
+        <v>454545</v>
       </c>
       <c r="F179">
         <v>7200</v>
@@ -4584,16 +4601,16 @@
         <v>178</v>
       </c>
       <c r="B180" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C180" s="6">
         <v>28800</v>
       </c>
       <c r="D180">
-        <v>82800</v>
+        <v>79200</v>
       </c>
       <c r="E180" s="6">
-        <v>400000</v>
+        <v>300000</v>
       </c>
       <c r="F180">
         <v>7200</v>
@@ -4604,16 +4621,16 @@
         <v>179</v>
       </c>
       <c r="B181" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C181" s="6">
-        <v>19800</v>
+        <v>28800</v>
       </c>
       <c r="D181">
-        <v>46800</v>
+        <v>82800</v>
       </c>
       <c r="E181" s="6">
-        <v>60000</v>
+        <v>400000</v>
       </c>
       <c r="F181">
         <v>7200</v>
@@ -4624,10 +4641,10 @@
         <v>180</v>
       </c>
       <c r="B182" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C182" s="6">
-        <v>23400</v>
+        <v>19800</v>
       </c>
       <c r="D182">
         <v>46800</v>
@@ -4644,16 +4661,16 @@
         <v>181</v>
       </c>
       <c r="B183" t="s">
-        <v>186</v>
-      </c>
-      <c r="C183" s="7">
-        <v>39600</v>
-      </c>
-      <c r="D183" s="3">
-        <v>52200</v>
+        <v>185</v>
+      </c>
+      <c r="C183" s="6">
+        <v>23400</v>
+      </c>
+      <c r="D183">
+        <v>46800</v>
       </c>
       <c r="E183" s="6">
-        <v>250000</v>
+        <v>60000</v>
       </c>
       <c r="F183">
         <v>7200</v>
@@ -4664,16 +4681,16 @@
         <v>182</v>
       </c>
       <c r="B184" t="s">
-        <v>187</v>
-      </c>
-      <c r="C184" s="6">
+        <v>186</v>
+      </c>
+      <c r="C184" s="7">
         <v>39600</v>
       </c>
-      <c r="D184">
-        <v>81000</v>
+      <c r="D184" s="3">
+        <v>52200</v>
       </c>
       <c r="E184" s="6">
-        <v>181818</v>
+        <v>250000</v>
       </c>
       <c r="F184">
         <v>7200</v>
@@ -4684,16 +4701,16 @@
         <v>183</v>
       </c>
       <c r="B185" t="s">
-        <v>188</v>
-      </c>
-      <c r="C185" s="7">
-        <v>36000</v>
-      </c>
-      <c r="D185" s="3">
-        <v>50400</v>
+        <v>187</v>
+      </c>
+      <c r="C185" s="6">
+        <v>39600</v>
+      </c>
+      <c r="D185">
+        <v>81000</v>
       </c>
       <c r="E185" s="6">
-        <v>200000</v>
+        <v>181818</v>
       </c>
       <c r="F185">
         <v>7200</v>
@@ -4704,16 +4721,16 @@
         <v>184</v>
       </c>
       <c r="B186" t="s">
-        <v>189</v>
-      </c>
-      <c r="C186" s="6">
-        <v>21600</v>
-      </c>
-      <c r="D186">
-        <v>79200</v>
+        <v>188</v>
+      </c>
+      <c r="C186" s="7">
+        <v>36000</v>
+      </c>
+      <c r="D186" s="3">
+        <v>50400</v>
       </c>
       <c r="E186" s="6">
-        <v>800000</v>
+        <v>200000</v>
       </c>
       <c r="F186">
         <v>7200</v>
@@ -4724,16 +4741,16 @@
         <v>185</v>
       </c>
       <c r="B187" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C187" s="6">
-        <v>32400</v>
+        <v>21600</v>
       </c>
       <c r="D187">
         <v>79200</v>
       </c>
       <c r="E187" s="6">
-        <v>750000</v>
+        <v>800000</v>
       </c>
       <c r="F187">
         <v>7200</v>
@@ -4744,16 +4761,16 @@
         <v>186</v>
       </c>
       <c r="B188" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C188" s="6">
         <v>32400</v>
       </c>
       <c r="D188">
-        <v>82800</v>
+        <v>79200</v>
       </c>
       <c r="E188" s="6">
-        <v>200000</v>
+        <v>750000</v>
       </c>
       <c r="F188">
         <v>7200</v>
@@ -4764,16 +4781,16 @@
         <v>187</v>
       </c>
       <c r="B189" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C189" s="6">
-        <v>21600</v>
+        <v>32400</v>
       </c>
       <c r="D189">
-        <v>43200</v>
+        <v>82800</v>
       </c>
       <c r="E189" s="6">
-        <v>30000</v>
+        <v>200000</v>
       </c>
       <c r="F189">
         <v>7200</v>
@@ -4784,18 +4801,38 @@
         <v>188</v>
       </c>
       <c r="B190" t="s">
+        <v>192</v>
+      </c>
+      <c r="C190" s="6">
+        <v>21600</v>
+      </c>
+      <c r="D190">
+        <v>43200</v>
+      </c>
+      <c r="E190" s="6">
+        <v>30000</v>
+      </c>
+      <c r="F190">
+        <v>7200</v>
+      </c>
+    </row>
+    <row r="191" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A191" s="1">
+        <v>189</v>
+      </c>
+      <c r="B191" t="s">
         <v>193</v>
       </c>
-      <c r="C190" s="6">
+      <c r="C191" s="6">
         <v>25200</v>
       </c>
-      <c r="D190">
-        <v>79200</v>
-      </c>
-      <c r="E190" s="6">
+      <c r="D191">
+        <v>79200</v>
+      </c>
+      <c r="E191" s="6">
         <v>250000</v>
       </c>
-      <c r="F190">
+      <c r="F191">
         <v>7200</v>
       </c>
     </row>

</xml_diff>